<commit_message>
Inner and outer insulation models
</commit_message>
<xml_diff>
--- a/svg/bridge_plain.dimensions.xlsx
+++ b/svg/bridge_plain.dimensions.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Compute values for 100 x 97 image used in equation system</t>
   </si>
   <si>
-    <t xml:space="preserve">Results are input for bridge_plain.png.csv</t>
+    <t xml:space="preserve">Results are input for bridge_plain.png.csv and other conductivity mapping  CSV files.</t>
   </si>
   <si>
     <t xml:space="preserve">Rows</t>
@@ -46,16 +46,16 @@
     <t xml:space="preserve">R_se</t>
   </si>
   <si>
+    <t xml:space="preserve">Lambda_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air-Inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_si</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lambda_i</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air-Inside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_si</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lambda_e</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>